<commit_message>
Updated Downtime tables so that they are dynamically readable in python. This will be used to create or update the hashmaps needed in javascript to make a bot that can resolve the more complex downtimes involving rolls.
</commit_message>
<xml_diff>
--- a/Downtimes/Westmarch tables.xlsx
+++ b/Downtimes/Westmarch tables.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederic\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frederic\Desktop\DnD Campaign\The Storm\Westmarch stuff\Westmarch-Trader\Downtimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB6EE421-04E9-4FCE-9E06-5D617FEBD83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DA7C02-FAA5-47F0-BD23-EAF95C20A29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-2445" windowWidth="16440" windowHeight="28440" xr2:uid="{D4D009D0-E6CD-4F99-8833-72BCD0A321B8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Session Rewards" sheetId="2" r:id="rId1"/>
-    <sheet name="Downtime" sheetId="1" r:id="rId2"/>
+    <sheet name="Downtime" sheetId="1" r:id="rId1"/>
+    <sheet name="Session Rewards" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="118">
   <si>
     <t>Job downtime</t>
   </si>
@@ -394,6 +394,21 @@
   </si>
   <si>
     <t>Minutes played</t>
+  </si>
+  <si>
+    <t>min roll</t>
+  </si>
+  <si>
+    <t>max roll</t>
+  </si>
+  <si>
+    <t>level start</t>
+  </si>
+  <si>
+    <t>max level</t>
+  </si>
+  <si>
+    <t>Ranges (for python)</t>
   </si>
 </sst>
 </file>
@@ -872,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1175,6 +1190,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1187,21 +1262,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1220,51 +1280,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1283,66 +1303,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>22713</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>70338</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="65" cy="172227"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B33244-0570-446C-901F-C7048D41B415}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8861913" y="3394563"/>
-          <a:ext cx="65" cy="172227"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1457,8 +1417,64 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>22713</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>70338</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22B33244-0570-446C-901F-C7048D41B415}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8861913" y="3394563"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1777,718 +1793,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E7EDF7-D003-493B-A466-C93A8A69CC27}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47"/>
-      <c r="D1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" s="136" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="128" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="52" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="I2" s="52" t="s">
-        <v>110</v>
-      </c>
-      <c r="K2" s="52" t="s">
-        <v>111</v>
-      </c>
-      <c r="L2" s="52" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55">
-        <v>2</v>
-      </c>
-      <c r="B3" s="58">
-        <v>900</v>
-      </c>
-      <c r="C3" s="56">
-        <v>600</v>
-      </c>
-      <c r="D3" s="132">
-        <v>1</v>
-      </c>
-      <c r="E3" s="56">
-        <f t="shared" ref="E3:E7" si="0">_xlfn.CEILING.MATH(C3/D3)</f>
-        <v>600</v>
-      </c>
-      <c r="G3" s="18">
-        <v>2</v>
-      </c>
-      <c r="H3" s="20">
-        <f>M6</f>
-        <v>100</v>
-      </c>
-      <c r="I3" s="20">
-        <f t="shared" ref="I3:I21" si="1">_xlfn.CEILING.MATH(H3*($K$3+$L$3/60))</f>
-        <v>400</v>
-      </c>
-      <c r="K3" s="134">
-        <v>4</v>
-      </c>
-      <c r="L3" s="135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="92">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="127">
-        <v>2700</v>
-      </c>
-      <c r="C4" s="61">
-        <f t="shared" ref="C4:C20" si="2">B4-B3</f>
-        <v>1800</v>
-      </c>
-      <c r="D4" s="131">
-        <v>2</v>
-      </c>
-      <c r="E4" s="61">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="G4" s="23">
-        <f>G3+1</f>
-        <v>3</v>
-      </c>
-      <c r="H4" s="25">
-        <f t="shared" ref="H4:H21" si="3">H3+M$7+M$8*(ROW()-3)</f>
-        <v>150</v>
-      </c>
-      <c r="I4" s="25">
-        <f t="shared" si="1"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68">
-        <f t="shared" ref="A5:A20" si="4">A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="71">
-        <v>6500</v>
-      </c>
-      <c r="C5" s="69">
-        <f t="shared" si="2"/>
-        <v>3800</v>
-      </c>
-      <c r="D5" s="133">
-        <v>4</v>
-      </c>
-      <c r="E5" s="69">
-        <f t="shared" si="0"/>
-        <v>950</v>
-      </c>
-      <c r="G5" s="31">
-        <f t="shared" ref="G5:G20" si="5">G4+1</f>
-        <v>4</v>
-      </c>
-      <c r="H5" s="33">
-        <f t="shared" si="3"/>
-        <v>200</v>
-      </c>
-      <c r="I5" s="33">
-        <f t="shared" si="1"/>
-        <v>800</v>
-      </c>
-      <c r="K5" s="138" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="139"/>
-      <c r="M5" s="140"/>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="92">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="127">
-        <v>14000</v>
-      </c>
-      <c r="C6" s="61">
-        <f t="shared" si="2"/>
-        <v>7500</v>
-      </c>
-      <c r="D6" s="131">
-        <v>6</v>
-      </c>
-      <c r="E6" s="61">
-        <f t="shared" si="0"/>
-        <v>1250</v>
-      </c>
-      <c r="G6" s="23">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="H6" s="25">
-        <f t="shared" si="3"/>
-        <v>250</v>
-      </c>
-      <c r="I6" s="25">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="K6" s="141" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="142"/>
-      <c r="M6" s="137">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="68">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="71">
-        <v>23000</v>
-      </c>
-      <c r="C7" s="69">
-        <f t="shared" si="2"/>
-        <v>9000</v>
-      </c>
-      <c r="D7" s="133">
-        <v>6</v>
-      </c>
-      <c r="E7" s="69">
-        <f t="shared" si="0"/>
-        <v>1500</v>
-      </c>
-      <c r="G7" s="31">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="H7" s="33">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-      <c r="I7" s="33">
-        <f t="shared" si="1"/>
-        <v>1200</v>
-      </c>
-      <c r="K7" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="144"/>
-      <c r="M7" s="38">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="92">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="127">
-        <v>34000</v>
-      </c>
-      <c r="C8" s="61">
-        <f t="shared" si="2"/>
-        <v>11000</v>
-      </c>
-      <c r="D8" s="131">
-        <v>7</v>
-      </c>
-      <c r="E8" s="61">
-        <f>_xlfn.CEILING.MATH(C8/D8)</f>
-        <v>1572</v>
-      </c>
-      <c r="G8" s="23">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="H8" s="25">
-        <f t="shared" si="3"/>
-        <v>350</v>
-      </c>
-      <c r="I8" s="25">
-        <f t="shared" si="1"/>
-        <v>1400</v>
-      </c>
-      <c r="K8" s="145" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="146"/>
-      <c r="M8" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="68">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="71">
-        <v>48000</v>
-      </c>
-      <c r="C9" s="69">
-        <f t="shared" si="2"/>
-        <v>14000</v>
-      </c>
-      <c r="D9" s="133">
-        <v>8</v>
-      </c>
-      <c r="E9" s="69">
-        <f t="shared" ref="E9:E20" si="6">_xlfn.CEILING.MATH(C9/D9)</f>
-        <v>1750</v>
-      </c>
-      <c r="G9" s="31">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="H9" s="33">
-        <f t="shared" si="3"/>
-        <v>400</v>
-      </c>
-      <c r="I9" s="33">
-        <f t="shared" si="1"/>
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="92">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="127">
-        <v>64000</v>
-      </c>
-      <c r="C10" s="61">
-        <f t="shared" si="2"/>
-        <v>16000</v>
-      </c>
-      <c r="D10" s="131">
-        <v>9</v>
-      </c>
-      <c r="E10" s="61">
-        <f t="shared" si="6"/>
-        <v>1778</v>
-      </c>
-      <c r="G10" s="23">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="H10" s="25">
-        <f t="shared" si="3"/>
-        <v>450</v>
-      </c>
-      <c r="I10" s="25">
-        <f t="shared" si="1"/>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="68">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="71">
-        <v>85000</v>
-      </c>
-      <c r="C11" s="69">
-        <f t="shared" si="2"/>
-        <v>21000</v>
-      </c>
-      <c r="D11" s="133">
-        <v>12</v>
-      </c>
-      <c r="E11" s="69">
-        <f t="shared" si="6"/>
-        <v>1750</v>
-      </c>
-      <c r="G11" s="31">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="H11" s="33">
-        <f t="shared" si="3"/>
-        <v>500</v>
-      </c>
-      <c r="I11" s="33">
-        <f t="shared" si="1"/>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="92">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="127">
-        <v>100000</v>
-      </c>
-      <c r="C12" s="61">
-        <f t="shared" si="2"/>
-        <v>15000</v>
-      </c>
-      <c r="D12" s="131">
-        <v>8</v>
-      </c>
-      <c r="E12" s="61">
-        <f t="shared" si="6"/>
-        <v>1875</v>
-      </c>
-      <c r="G12" s="23">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="H12" s="25">
-        <f t="shared" si="3"/>
-        <v>550</v>
-      </c>
-      <c r="I12" s="25">
-        <f t="shared" si="1"/>
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="68">
-        <f t="shared" si="4"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="71">
-        <v>120000</v>
-      </c>
-      <c r="C13" s="69">
-        <f t="shared" si="2"/>
-        <v>20000</v>
-      </c>
-      <c r="D13" s="133">
-        <v>10</v>
-      </c>
-      <c r="E13" s="69">
-        <f t="shared" si="6"/>
-        <v>2000</v>
-      </c>
-      <c r="G13" s="31">
-        <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="H13" s="33">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-      <c r="I13" s="33">
-        <f t="shared" si="1"/>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="92">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="127">
-        <v>140000</v>
-      </c>
-      <c r="C14" s="61">
-        <f t="shared" si="2"/>
-        <v>20000</v>
-      </c>
-      <c r="D14" s="131">
-        <v>9</v>
-      </c>
-      <c r="E14" s="61">
-        <f t="shared" si="6"/>
-        <v>2223</v>
-      </c>
-      <c r="G14" s="23">
-        <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="H14" s="25">
-        <f t="shared" si="3"/>
-        <v>650</v>
-      </c>
-      <c r="I14" s="25">
-        <f t="shared" si="1"/>
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="68">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="71">
-        <v>165000</v>
-      </c>
-      <c r="C15" s="69">
-        <f t="shared" si="2"/>
-        <v>25000</v>
-      </c>
-      <c r="D15" s="133">
-        <v>10</v>
-      </c>
-      <c r="E15" s="69">
-        <f t="shared" si="6"/>
-        <v>2500</v>
-      </c>
-      <c r="G15" s="31">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="H15" s="33">
-        <f t="shared" si="3"/>
-        <v>700</v>
-      </c>
-      <c r="I15" s="33">
-        <f t="shared" si="1"/>
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="92">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="127">
-        <v>195000</v>
-      </c>
-      <c r="C16" s="61">
-        <f t="shared" si="2"/>
-        <v>30000</v>
-      </c>
-      <c r="D16" s="131">
-        <v>12</v>
-      </c>
-      <c r="E16" s="61">
-        <f t="shared" si="6"/>
-        <v>2500</v>
-      </c>
-      <c r="G16" s="23">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="H16" s="25">
-        <f t="shared" si="3"/>
-        <v>750</v>
-      </c>
-      <c r="I16" s="25">
-        <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="68">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="71">
-        <v>225000</v>
-      </c>
-      <c r="C17" s="69">
-        <f t="shared" si="2"/>
-        <v>30000</v>
-      </c>
-      <c r="D17" s="133">
-        <v>11</v>
-      </c>
-      <c r="E17" s="69">
-        <f t="shared" si="6"/>
-        <v>2728</v>
-      </c>
-      <c r="G17" s="31">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="H17" s="33">
-        <f t="shared" si="3"/>
-        <v>800</v>
-      </c>
-      <c r="I17" s="33">
-        <f t="shared" si="1"/>
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="92">
-        <f t="shared" si="4"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="127">
-        <v>265000</v>
-      </c>
-      <c r="C18" s="61">
-        <f t="shared" si="2"/>
-        <v>40000</v>
-      </c>
-      <c r="D18" s="131">
-        <v>12</v>
-      </c>
-      <c r="E18" s="61">
-        <f t="shared" si="6"/>
-        <v>3334</v>
-      </c>
-      <c r="G18" s="23">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="H18" s="25">
-        <f t="shared" si="3"/>
-        <v>850</v>
-      </c>
-      <c r="I18" s="25">
-        <f t="shared" si="1"/>
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="68">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="71">
-        <v>305000</v>
-      </c>
-      <c r="C19" s="69">
-        <f t="shared" si="2"/>
-        <v>40000</v>
-      </c>
-      <c r="D19" s="133">
-        <v>11</v>
-      </c>
-      <c r="E19" s="69">
-        <f t="shared" si="6"/>
-        <v>3637</v>
-      </c>
-      <c r="G19" s="31">
-        <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="H19" s="33">
-        <f t="shared" si="3"/>
-        <v>900</v>
-      </c>
-      <c r="I19" s="33">
-        <f t="shared" si="1"/>
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="92">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="127">
-        <v>355000</v>
-      </c>
-      <c r="C20" s="61">
-        <f t="shared" si="2"/>
-        <v>50000</v>
-      </c>
-      <c r="D20" s="131">
-        <v>11</v>
-      </c>
-      <c r="E20" s="61">
-        <f t="shared" si="6"/>
-        <v>4546</v>
-      </c>
-      <c r="G20" s="23">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="H20" s="25">
-        <f t="shared" si="3"/>
-        <v>950</v>
-      </c>
-      <c r="I20" s="25">
-        <f t="shared" si="1"/>
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105">
-        <f>A20+1</f>
-        <v>20</v>
-      </c>
-      <c r="B21" s="129" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="126" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="130" t="str">
-        <f>"Total = "&amp;SUM(D3:D20)</f>
-        <v>Total = 149</v>
-      </c>
-      <c r="E21" s="126"/>
-      <c r="G21" s="40">
-        <f>G20+1</f>
-        <v>20</v>
-      </c>
-      <c r="H21" s="42">
-        <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="I21" s="42">
-        <f t="shared" si="1"/>
-        <v>4000</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7131BC77-EA3F-4250-B65F-AF333CED2AC2}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AF117"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,10 +1820,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="156"/>
+      <c r="B1" s="163"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="6" t="s">
@@ -2625,22 +1935,22 @@
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="173"/>
+      <c r="C3" s="167"/>
       <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="172"/>
-      <c r="G3" s="172"/>
-      <c r="H3" s="172"/>
-      <c r="I3" s="172"/>
-      <c r="J3" s="172"/>
-      <c r="K3" s="173"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="167"/>
       <c r="L3" s="138" t="s">
         <v>64</v>
       </c>
@@ -2709,10 +2019,10 @@
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
-      <c r="L4" s="157" t="s">
+      <c r="L4" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="M4" s="158"/>
+      <c r="M4" s="169"/>
       <c r="N4" s="22">
         <v>0.1</v>
       </c>
@@ -3797,7 +3107,7 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -3851,12 +3161,16 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
+      <c r="S20" s="2">
+        <f>COLUMN()</f>
+        <v>19</v>
+      </c>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
+      <c r="X20" s="2">
+        <f>COLUMN()</f>
+        <v>24</v>
+      </c>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -3866,7 +3180,7 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
     </row>
-    <row r="21" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -3919,13 +3233,22 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
+      <c r="S21" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
+      <c r="U21" s="181" t="s">
+        <v>113</v>
+      </c>
+      <c r="V21" s="181" t="s">
+        <v>114</v>
+      </c>
+      <c r="W21" s="181" t="s">
+        <v>115</v>
+      </c>
+      <c r="X21" s="181" t="s">
+        <v>116</v>
+      </c>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
@@ -3988,13 +3311,26 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
+      <c r="R22" s="2">
+        <f>ROW()</f>
+        <v>22</v>
+      </c>
+      <c r="S22" s="162" t="s">
+        <v>0</v>
+      </c>
+      <c r="T22" s="164"/>
+      <c r="U22" s="116">
+        <v>2</v>
+      </c>
+      <c r="V22" s="116">
+        <v>11</v>
+      </c>
+      <c r="W22" s="116">
+        <v>3</v>
+      </c>
+      <c r="X22" s="116">
+        <v>22</v>
+      </c>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
@@ -4004,7 +3340,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4023,12 +3359,22 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
+      <c r="S23" s="162" t="s">
+        <v>23</v>
+      </c>
+      <c r="T23" s="164"/>
+      <c r="U23" s="182">
+        <v>4</v>
+      </c>
+      <c r="V23" s="182">
+        <v>13</v>
+      </c>
+      <c r="W23" s="182">
+        <v>27</v>
+      </c>
+      <c r="X23" s="182">
+        <v>45</v>
+      </c>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
@@ -4057,12 +3403,22 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
-      <c r="X24" s="2"/>
+      <c r="S24" s="170" t="s">
+        <v>92</v>
+      </c>
+      <c r="T24" s="180"/>
+      <c r="U24" s="116">
+        <v>4</v>
+      </c>
+      <c r="V24" s="116">
+        <v>13</v>
+      </c>
+      <c r="W24" s="116">
+        <v>85</v>
+      </c>
+      <c r="X24" s="116">
+        <v>104</v>
+      </c>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
@@ -4073,10 +3429,10 @@
       <c r="AF24" s="2"/>
     </row>
     <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="154" t="s">
+      <c r="A25" s="162" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="156"/>
+      <c r="B25" s="163"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -4205,15 +3561,15 @@
       <c r="F27" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="171" t="s">
+      <c r="G27" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="172"/>
-      <c r="I27" s="172"/>
-      <c r="J27" s="172"/>
-      <c r="K27" s="172"/>
-      <c r="L27" s="172"/>
-      <c r="M27" s="172"/>
+      <c r="H27" s="166"/>
+      <c r="I27" s="166"/>
+      <c r="J27" s="166"/>
+      <c r="K27" s="166"/>
+      <c r="L27" s="166"/>
+      <c r="M27" s="166"/>
       <c r="N27" s="53" t="s">
         <v>31</v>
       </c>
@@ -5579,11 +4935,11 @@
       <c r="AF47" s="2"/>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A48" s="154" t="s">
+      <c r="A48" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="155"/>
-      <c r="C48" s="156"/>
+      <c r="B48" s="164"/>
+      <c r="C48" s="163"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -5615,18 +4971,18 @@
       <c r="AF48" s="2"/>
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A49" s="153" t="s">
+      <c r="A49" s="173" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="153"/>
-      <c r="C49" s="153"/>
-      <c r="D49" s="153"/>
-      <c r="E49" s="153"/>
-      <c r="F49" s="153"/>
-      <c r="G49" s="153"/>
-      <c r="H49" s="153"/>
-      <c r="I49" s="153"/>
-      <c r="J49" s="153"/>
+      <c r="B49" s="173"/>
+      <c r="C49" s="173"/>
+      <c r="D49" s="173"/>
+      <c r="E49" s="173"/>
+      <c r="F49" s="173"/>
+      <c r="G49" s="173"/>
+      <c r="H49" s="173"/>
+      <c r="I49" s="173"/>
+      <c r="J49" s="173"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
@@ -5654,22 +5010,22 @@
       <c r="A50" s="80">
         <v>1</v>
       </c>
-      <c r="B50" s="174" t="s">
+      <c r="B50" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="175"/>
-      <c r="D50" s="175"/>
-      <c r="E50" s="175"/>
-      <c r="F50" s="175"/>
-      <c r="G50" s="175"/>
-      <c r="H50" s="175"/>
-      <c r="I50" s="175"/>
-      <c r="J50" s="175"/>
-      <c r="K50" s="175"/>
-      <c r="L50" s="175"/>
-      <c r="M50" s="175"/>
-      <c r="N50" s="175"/>
-      <c r="O50" s="176"/>
+      <c r="C50" s="151"/>
+      <c r="D50" s="151"/>
+      <c r="E50" s="151"/>
+      <c r="F50" s="151"/>
+      <c r="G50" s="151"/>
+      <c r="H50" s="151"/>
+      <c r="I50" s="151"/>
+      <c r="J50" s="151"/>
+      <c r="K50" s="151"/>
+      <c r="L50" s="151"/>
+      <c r="M50" s="151"/>
+      <c r="N50" s="151"/>
+      <c r="O50" s="152"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
@@ -5692,22 +5048,22 @@
       <c r="A51" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="168" t="s">
+      <c r="B51" s="159" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="169"/>
-      <c r="D51" s="169"/>
-      <c r="E51" s="169"/>
-      <c r="F51" s="169"/>
-      <c r="G51" s="169"/>
-      <c r="H51" s="169"/>
-      <c r="I51" s="169"/>
-      <c r="J51" s="169"/>
-      <c r="K51" s="169"/>
-      <c r="L51" s="169"/>
-      <c r="M51" s="169"/>
-      <c r="N51" s="169"/>
-      <c r="O51" s="170"/>
+      <c r="C51" s="160"/>
+      <c r="D51" s="160"/>
+      <c r="E51" s="160"/>
+      <c r="F51" s="160"/>
+      <c r="G51" s="160"/>
+      <c r="H51" s="160"/>
+      <c r="I51" s="160"/>
+      <c r="J51" s="160"/>
+      <c r="K51" s="160"/>
+      <c r="L51" s="160"/>
+      <c r="M51" s="160"/>
+      <c r="N51" s="160"/>
+      <c r="O51" s="161"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
@@ -5730,22 +5086,22 @@
       <c r="A52" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="B52" s="165" t="s">
+      <c r="B52" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="166"/>
-      <c r="D52" s="166"/>
-      <c r="E52" s="166"/>
-      <c r="F52" s="166"/>
-      <c r="G52" s="166"/>
-      <c r="H52" s="166"/>
-      <c r="I52" s="166"/>
-      <c r="J52" s="166"/>
-      <c r="K52" s="166"/>
-      <c r="L52" s="166"/>
-      <c r="M52" s="166"/>
-      <c r="N52" s="166"/>
-      <c r="O52" s="167"/>
+      <c r="C52" s="157"/>
+      <c r="D52" s="157"/>
+      <c r="E52" s="157"/>
+      <c r="F52" s="157"/>
+      <c r="G52" s="157"/>
+      <c r="H52" s="157"/>
+      <c r="I52" s="157"/>
+      <c r="J52" s="157"/>
+      <c r="K52" s="157"/>
+      <c r="L52" s="157"/>
+      <c r="M52" s="157"/>
+      <c r="N52" s="157"/>
+      <c r="O52" s="158"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
@@ -5768,22 +5124,22 @@
       <c r="A53" s="83">
         <v>51</v>
       </c>
-      <c r="B53" s="168" t="s">
+      <c r="B53" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="169"/>
-      <c r="D53" s="169"/>
-      <c r="E53" s="169"/>
-      <c r="F53" s="169"/>
-      <c r="G53" s="169"/>
-      <c r="H53" s="169"/>
-      <c r="I53" s="169"/>
-      <c r="J53" s="169"/>
-      <c r="K53" s="169"/>
-      <c r="L53" s="169"/>
-      <c r="M53" s="169"/>
-      <c r="N53" s="169"/>
-      <c r="O53" s="170"/>
+      <c r="C53" s="160"/>
+      <c r="D53" s="160"/>
+      <c r="E53" s="160"/>
+      <c r="F53" s="160"/>
+      <c r="G53" s="160"/>
+      <c r="H53" s="160"/>
+      <c r="I53" s="160"/>
+      <c r="J53" s="160"/>
+      <c r="K53" s="160"/>
+      <c r="L53" s="160"/>
+      <c r="M53" s="160"/>
+      <c r="N53" s="160"/>
+      <c r="O53" s="161"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
@@ -5806,22 +5162,22 @@
       <c r="A54" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="165" t="s">
+      <c r="B54" s="156" t="s">
         <v>43</v>
       </c>
-      <c r="C54" s="166"/>
-      <c r="D54" s="166"/>
-      <c r="E54" s="166"/>
-      <c r="F54" s="166"/>
-      <c r="G54" s="166"/>
-      <c r="H54" s="166"/>
-      <c r="I54" s="166"/>
-      <c r="J54" s="166"/>
-      <c r="K54" s="166"/>
-      <c r="L54" s="166"/>
-      <c r="M54" s="166"/>
-      <c r="N54" s="166"/>
-      <c r="O54" s="167"/>
+      <c r="C54" s="157"/>
+      <c r="D54" s="157"/>
+      <c r="E54" s="157"/>
+      <c r="F54" s="157"/>
+      <c r="G54" s="157"/>
+      <c r="H54" s="157"/>
+      <c r="I54" s="157"/>
+      <c r="J54" s="157"/>
+      <c r="K54" s="157"/>
+      <c r="L54" s="157"/>
+      <c r="M54" s="157"/>
+      <c r="N54" s="157"/>
+      <c r="O54" s="158"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
@@ -5844,22 +5200,22 @@
       <c r="A55" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="168" t="s">
+      <c r="B55" s="159" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="169"/>
-      <c r="D55" s="169"/>
-      <c r="E55" s="169"/>
-      <c r="F55" s="169"/>
-      <c r="G55" s="169"/>
-      <c r="H55" s="169"/>
-      <c r="I55" s="169"/>
-      <c r="J55" s="169"/>
-      <c r="K55" s="169"/>
-      <c r="L55" s="169"/>
-      <c r="M55" s="169"/>
-      <c r="N55" s="169"/>
-      <c r="O55" s="170"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="160"/>
+      <c r="E55" s="160"/>
+      <c r="F55" s="160"/>
+      <c r="G55" s="160"/>
+      <c r="H55" s="160"/>
+      <c r="I55" s="160"/>
+      <c r="J55" s="160"/>
+      <c r="K55" s="160"/>
+      <c r="L55" s="160"/>
+      <c r="M55" s="160"/>
+      <c r="N55" s="160"/>
+      <c r="O55" s="161"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
@@ -5882,22 +5238,22 @@
       <c r="A56" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="165" t="s">
+      <c r="B56" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="C56" s="166"/>
-      <c r="D56" s="166"/>
-      <c r="E56" s="166"/>
-      <c r="F56" s="166"/>
-      <c r="G56" s="166"/>
-      <c r="H56" s="166"/>
-      <c r="I56" s="166"/>
-      <c r="J56" s="166"/>
-      <c r="K56" s="166"/>
-      <c r="L56" s="166"/>
-      <c r="M56" s="166"/>
-      <c r="N56" s="166"/>
-      <c r="O56" s="167"/>
+      <c r="C56" s="157"/>
+      <c r="D56" s="157"/>
+      <c r="E56" s="157"/>
+      <c r="F56" s="157"/>
+      <c r="G56" s="157"/>
+      <c r="H56" s="157"/>
+      <c r="I56" s="157"/>
+      <c r="J56" s="157"/>
+      <c r="K56" s="157"/>
+      <c r="L56" s="157"/>
+      <c r="M56" s="157"/>
+      <c r="N56" s="157"/>
+      <c r="O56" s="158"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
@@ -5920,22 +5276,22 @@
       <c r="A57" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="168" t="s">
+      <c r="B57" s="159" t="s">
         <v>46</v>
       </c>
-      <c r="C57" s="169"/>
-      <c r="D57" s="169"/>
-      <c r="E57" s="169"/>
-      <c r="F57" s="169"/>
-      <c r="G57" s="169"/>
-      <c r="H57" s="169"/>
-      <c r="I57" s="169"/>
-      <c r="J57" s="169"/>
-      <c r="K57" s="169"/>
-      <c r="L57" s="169"/>
-      <c r="M57" s="169"/>
-      <c r="N57" s="169"/>
-      <c r="O57" s="170"/>
+      <c r="C57" s="160"/>
+      <c r="D57" s="160"/>
+      <c r="E57" s="160"/>
+      <c r="F57" s="160"/>
+      <c r="G57" s="160"/>
+      <c r="H57" s="160"/>
+      <c r="I57" s="160"/>
+      <c r="J57" s="160"/>
+      <c r="K57" s="160"/>
+      <c r="L57" s="160"/>
+      <c r="M57" s="160"/>
+      <c r="N57" s="160"/>
+      <c r="O57" s="161"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
@@ -5958,22 +5314,22 @@
       <c r="A58" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="162" t="s">
+      <c r="B58" s="177" t="s">
         <v>47</v>
       </c>
-      <c r="C58" s="163"/>
-      <c r="D58" s="163"/>
-      <c r="E58" s="163"/>
-      <c r="F58" s="163"/>
-      <c r="G58" s="163"/>
-      <c r="H58" s="163"/>
-      <c r="I58" s="163"/>
-      <c r="J58" s="163"/>
-      <c r="K58" s="163"/>
-      <c r="L58" s="163"/>
-      <c r="M58" s="163"/>
-      <c r="N58" s="163"/>
-      <c r="O58" s="164"/>
+      <c r="C58" s="178"/>
+      <c r="D58" s="178"/>
+      <c r="E58" s="178"/>
+      <c r="F58" s="178"/>
+      <c r="G58" s="178"/>
+      <c r="H58" s="178"/>
+      <c r="I58" s="178"/>
+      <c r="J58" s="178"/>
+      <c r="K58" s="178"/>
+      <c r="L58" s="178"/>
+      <c r="M58" s="178"/>
+      <c r="N58" s="178"/>
+      <c r="O58" s="179"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
@@ -6061,13 +5417,13 @@
       <c r="AF60" s="2"/>
     </row>
     <row r="61" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="154" t="s">
+      <c r="A61" s="162" t="s">
         <v>100</v>
       </c>
-      <c r="B61" s="155"/>
-      <c r="C61" s="155"/>
-      <c r="D61" s="155"/>
-      <c r="E61" s="156"/>
+      <c r="B61" s="164"/>
+      <c r="C61" s="164"/>
+      <c r="D61" s="164"/>
+      <c r="E61" s="163"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -6106,16 +5462,16 @@
       <c r="C62" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="160" t="s">
+      <c r="D62" s="175" t="s">
         <v>50</v>
       </c>
-      <c r="E62" s="161"/>
+      <c r="E62" s="176"/>
       <c r="F62" s="87"/>
-      <c r="G62" s="177" t="s">
+      <c r="G62" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="H62" s="178"/>
-      <c r="I62" s="179"/>
+      <c r="H62" s="154"/>
+      <c r="I62" s="155"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
@@ -6158,10 +5514,10 @@
         <v>63</v>
       </c>
       <c r="F63" s="90"/>
-      <c r="G63" s="157" t="s">
+      <c r="G63" s="168" t="s">
         <v>51</v>
       </c>
-      <c r="H63" s="158"/>
+      <c r="H63" s="169"/>
       <c r="I63" s="91">
         <v>4500</v>
       </c>
@@ -6706,7 +6062,7 @@
       <c r="G74" s="143" t="s">
         <v>59</v>
       </c>
-      <c r="H74" s="159"/>
+      <c r="H74" s="174"/>
       <c r="I74" s="96">
         <v>2</v>
       </c>
@@ -6758,7 +6114,7 @@
       <c r="G75" s="145" t="s">
         <v>61</v>
       </c>
-      <c r="H75" s="152"/>
+      <c r="H75" s="172"/>
       <c r="I75" s="102">
         <v>10</v>
       </c>
@@ -7133,10 +6489,10 @@
       <c r="AF83" s="2"/>
     </row>
     <row r="84" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="150" t="s">
+      <c r="A84" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="B84" s="151"/>
+      <c r="B84" s="171"/>
       <c r="C84" s="119" t="s">
         <v>3</v>
       </c>
@@ -8846,31 +8202,10 @@
       <c r="X117" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="B50:O50"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O28:Q28"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="B56:O56"/>
-    <mergeCell ref="B57:O57"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="G27:M27"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="E3:K3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="L4:M4"/>
+  <mergeCells count="43">
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S24:T24"/>
     <mergeCell ref="H85:M85"/>
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="G75:H75"/>
@@ -8887,6 +8222,30 @@
     <mergeCell ref="B52:O52"/>
     <mergeCell ref="B51:O51"/>
     <mergeCell ref="B55:O55"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="G27:M27"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="L14:N14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="E3:K3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="B50:O50"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O28:Q28"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="B56:O56"/>
+    <mergeCell ref="B57:O57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -8894,4 +8253,710 @@
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E7EDF7-D003-493B-A466-C93A8A69CC27}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:M21"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47"/>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="136" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="128" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="55">
+        <v>2</v>
+      </c>
+      <c r="B3" s="58">
+        <v>900</v>
+      </c>
+      <c r="C3" s="56">
+        <v>600</v>
+      </c>
+      <c r="D3" s="132">
+        <v>1</v>
+      </c>
+      <c r="E3" s="56">
+        <f t="shared" ref="E3:E7" si="0">_xlfn.CEILING.MATH(C3/D3)</f>
+        <v>600</v>
+      </c>
+      <c r="G3" s="18">
+        <v>2</v>
+      </c>
+      <c r="H3" s="20">
+        <f>M6</f>
+        <v>100</v>
+      </c>
+      <c r="I3" s="20">
+        <f t="shared" ref="I3:I21" si="1">_xlfn.CEILING.MATH(H3*($K$3+$L$3/60))</f>
+        <v>400</v>
+      </c>
+      <c r="K3" s="134">
+        <v>4</v>
+      </c>
+      <c r="L3" s="135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="92">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="127">
+        <v>2700</v>
+      </c>
+      <c r="C4" s="61">
+        <f t="shared" ref="C4:C20" si="2">B4-B3</f>
+        <v>1800</v>
+      </c>
+      <c r="D4" s="131">
+        <v>2</v>
+      </c>
+      <c r="E4" s="61">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="G4" s="23">
+        <f>G3+1</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="25">
+        <f t="shared" ref="H4:H21" si="3">H3+M$7+M$8*(ROW()-3)</f>
+        <v>150</v>
+      </c>
+      <c r="I4" s="25">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="68">
+        <f t="shared" ref="A5:A20" si="4">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="71">
+        <v>6500</v>
+      </c>
+      <c r="C5" s="69">
+        <f t="shared" si="2"/>
+        <v>3800</v>
+      </c>
+      <c r="D5" s="133">
+        <v>4</v>
+      </c>
+      <c r="E5" s="69">
+        <f t="shared" si="0"/>
+        <v>950</v>
+      </c>
+      <c r="G5" s="31">
+        <f t="shared" ref="G5:G20" si="5">G4+1</f>
+        <v>4</v>
+      </c>
+      <c r="H5" s="33">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="I5" s="33">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="K5" s="138" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="139"/>
+      <c r="M5" s="140"/>
+    </row>
+    <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="92">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="127">
+        <v>14000</v>
+      </c>
+      <c r="C6" s="61">
+        <f t="shared" si="2"/>
+        <v>7500</v>
+      </c>
+      <c r="D6" s="131">
+        <v>6</v>
+      </c>
+      <c r="E6" s="61">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="H6" s="25">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="I6" s="25">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="K6" s="141" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="142"/>
+      <c r="M6" s="137">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="68">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="71">
+        <v>23000</v>
+      </c>
+      <c r="C7" s="69">
+        <f t="shared" si="2"/>
+        <v>9000</v>
+      </c>
+      <c r="D7" s="133">
+        <v>6</v>
+      </c>
+      <c r="E7" s="69">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="G7" s="31">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="33">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="I7" s="33">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="K7" s="143" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="144"/>
+      <c r="M7" s="38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="92">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="127">
+        <v>34000</v>
+      </c>
+      <c r="C8" s="61">
+        <f t="shared" si="2"/>
+        <v>11000</v>
+      </c>
+      <c r="D8" s="131">
+        <v>7</v>
+      </c>
+      <c r="E8" s="61">
+        <f>_xlfn.CEILING.MATH(C8/D8)</f>
+        <v>1572</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="H8" s="25">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="I8" s="25">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="K8" s="145" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="146"/>
+      <c r="M8" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="68">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="71">
+        <v>48000</v>
+      </c>
+      <c r="C9" s="69">
+        <f t="shared" si="2"/>
+        <v>14000</v>
+      </c>
+      <c r="D9" s="133">
+        <v>8</v>
+      </c>
+      <c r="E9" s="69">
+        <f t="shared" ref="E9:E20" si="6">_xlfn.CEILING.MATH(C9/D9)</f>
+        <v>1750</v>
+      </c>
+      <c r="G9" s="31">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H9" s="33">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+      <c r="I9" s="33">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="92">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="127">
+        <v>64000</v>
+      </c>
+      <c r="C10" s="61">
+        <f t="shared" si="2"/>
+        <v>16000</v>
+      </c>
+      <c r="D10" s="131">
+        <v>9</v>
+      </c>
+      <c r="E10" s="61">
+        <f t="shared" si="6"/>
+        <v>1778</v>
+      </c>
+      <c r="G10" s="23">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="25">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="I10" s="25">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="68">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="71">
+        <v>85000</v>
+      </c>
+      <c r="C11" s="69">
+        <f t="shared" si="2"/>
+        <v>21000</v>
+      </c>
+      <c r="D11" s="133">
+        <v>12</v>
+      </c>
+      <c r="E11" s="69">
+        <f t="shared" si="6"/>
+        <v>1750</v>
+      </c>
+      <c r="G11" s="31">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="H11" s="33">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="I11" s="33">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="92">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="127">
+        <v>100000</v>
+      </c>
+      <c r="C12" s="61">
+        <f t="shared" si="2"/>
+        <v>15000</v>
+      </c>
+      <c r="D12" s="131">
+        <v>8</v>
+      </c>
+      <c r="E12" s="61">
+        <f t="shared" si="6"/>
+        <v>1875</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="H12" s="25">
+        <f t="shared" si="3"/>
+        <v>550</v>
+      </c>
+      <c r="I12" s="25">
+        <f t="shared" si="1"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="68">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="71">
+        <v>120000</v>
+      </c>
+      <c r="C13" s="69">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+      <c r="D13" s="133">
+        <v>10</v>
+      </c>
+      <c r="E13" s="69">
+        <f t="shared" si="6"/>
+        <v>2000</v>
+      </c>
+      <c r="G13" s="31">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="H13" s="33">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+      <c r="I13" s="33">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="92">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="127">
+        <v>140000</v>
+      </c>
+      <c r="C14" s="61">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+      <c r="D14" s="131">
+        <v>9</v>
+      </c>
+      <c r="E14" s="61">
+        <f t="shared" si="6"/>
+        <v>2223</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="H14" s="25">
+        <f t="shared" si="3"/>
+        <v>650</v>
+      </c>
+      <c r="I14" s="25">
+        <f t="shared" si="1"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="68">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="71">
+        <v>165000</v>
+      </c>
+      <c r="C15" s="69">
+        <f t="shared" si="2"/>
+        <v>25000</v>
+      </c>
+      <c r="D15" s="133">
+        <v>10</v>
+      </c>
+      <c r="E15" s="69">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="G15" s="31">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H15" s="33">
+        <f t="shared" si="3"/>
+        <v>700</v>
+      </c>
+      <c r="I15" s="33">
+        <f t="shared" si="1"/>
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="92">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="127">
+        <v>195000</v>
+      </c>
+      <c r="C16" s="61">
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+      <c r="D16" s="131">
+        <v>12</v>
+      </c>
+      <c r="E16" s="61">
+        <f t="shared" si="6"/>
+        <v>2500</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="H16" s="25">
+        <f t="shared" si="3"/>
+        <v>750</v>
+      </c>
+      <c r="I16" s="25">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="68">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="71">
+        <v>225000</v>
+      </c>
+      <c r="C17" s="69">
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+      <c r="D17" s="133">
+        <v>11</v>
+      </c>
+      <c r="E17" s="69">
+        <f t="shared" si="6"/>
+        <v>2728</v>
+      </c>
+      <c r="G17" s="31">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="H17" s="33">
+        <f t="shared" si="3"/>
+        <v>800</v>
+      </c>
+      <c r="I17" s="33">
+        <f t="shared" si="1"/>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="92">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="127">
+        <v>265000</v>
+      </c>
+      <c r="C18" s="61">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="D18" s="131">
+        <v>12</v>
+      </c>
+      <c r="E18" s="61">
+        <f t="shared" si="6"/>
+        <v>3334</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="H18" s="25">
+        <f t="shared" si="3"/>
+        <v>850</v>
+      </c>
+      <c r="I18" s="25">
+        <f t="shared" si="1"/>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="68">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="71">
+        <v>305000</v>
+      </c>
+      <c r="C19" s="69">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="D19" s="133">
+        <v>11</v>
+      </c>
+      <c r="E19" s="69">
+        <f t="shared" si="6"/>
+        <v>3637</v>
+      </c>
+      <c r="G19" s="31">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="H19" s="33">
+        <f t="shared" si="3"/>
+        <v>900</v>
+      </c>
+      <c r="I19" s="33">
+        <f t="shared" si="1"/>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="92">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="127">
+        <v>355000</v>
+      </c>
+      <c r="C20" s="61">
+        <f t="shared" si="2"/>
+        <v>50000</v>
+      </c>
+      <c r="D20" s="131">
+        <v>11</v>
+      </c>
+      <c r="E20" s="61">
+        <f t="shared" si="6"/>
+        <v>4546</v>
+      </c>
+      <c r="G20" s="23">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="H20" s="25">
+        <f t="shared" si="3"/>
+        <v>950</v>
+      </c>
+      <c r="I20" s="25">
+        <f t="shared" si="1"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="105">
+        <f>A20+1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="129" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" s="126" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="130" t="str">
+        <f>"Total = "&amp;SUM(D3:D20)</f>
+        <v>Total = 149</v>
+      </c>
+      <c r="E21" s="126"/>
+      <c r="G21" s="40">
+        <f>G20+1</f>
+        <v>20</v>
+      </c>
+      <c r="H21" s="42">
+        <f t="shared" si="3"/>
+        <v>1000</v>
+      </c>
+      <c r="I21" s="42">
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>